<commit_message>
L099, L101, L102 annotations updated and tsv extractions made
</commit_message>
<xml_diff>
--- a/exports/L098-tok-result-teiDict2tsv-corpus2TEIDict.xlsx
+++ b/exports/L098-tok-result-teiDict2tsv-corpus2TEIDict.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbowers\Desktop\Mixtepec_Mixtec\exports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackbowers/Box Sync/Language_Data/Mixtepec_Mixtec/exports/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0CD4A9-EAFD-014B-A61A-C0E3A4DE0739}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21945" windowHeight="10830"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="26320" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,8 +28,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="L098-tok-result-csv" type="6" refreshedVersion="5" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="L098-tok-result-csv" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\jbowers\Desktop\Mixtepec_Mixtec\exports\L098-tok-result-csv.txt">
       <textFields count="13">
         <textField/>
@@ -1430,8 +1431,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1442,6 +1443,30 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1476,15 +1501,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1500,7 +1528,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="L098-tok-result-csv" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="L098-tok-result-csv" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1765,30 +1793,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="63.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="63.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="81.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="70" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1826,7 +1854,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1850,7 +1878,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>388</v>
       </c>
@@ -1876,7 +1904,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>389</v>
       </c>
@@ -1899,7 +1927,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>390</v>
       </c>
@@ -1913,7 +1941,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>391</v>
       </c>
@@ -1933,7 +1961,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>392</v>
       </c>
@@ -1953,7 +1981,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1973,7 +2001,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>393</v>
       </c>
@@ -1993,7 +2021,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>394</v>
       </c>
@@ -2025,7 +2053,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>395</v>
       </c>
@@ -2045,7 +2073,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>396</v>
       </c>
@@ -2065,27 +2093,27 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>397</v>
       </c>
@@ -2114,7 +2142,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>398</v>
       </c>
@@ -2134,7 +2162,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>399</v>
       </c>
@@ -2154,7 +2182,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>399</v>
       </c>
@@ -2174,7 +2202,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>400</v>
       </c>
@@ -2194,7 +2222,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>401</v>
       </c>
@@ -2217,7 +2245,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>402</v>
       </c>
@@ -2237,7 +2265,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>403</v>
       </c>
@@ -2257,7 +2285,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>404</v>
       </c>
@@ -2277,7 +2305,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>405</v>
       </c>
@@ -2300,7 +2328,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>108</v>
       </c>
@@ -2320,7 +2348,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>113</v>
       </c>
@@ -2340,7 +2368,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>406</v>
       </c>
@@ -2360,7 +2388,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>407</v>
       </c>
@@ -2380,7 +2408,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>398</v>
       </c>
@@ -2400,7 +2428,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>405</v>
       </c>
@@ -2423,7 +2451,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>408</v>
       </c>
@@ -2443,27 +2471,27 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="L31" t="s">
+      <c r="L31" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>131</v>
       </c>
@@ -2483,27 +2511,27 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K33" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="L33" t="s">
+      <c r="L33" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>405</v>
       </c>
@@ -2526,7 +2554,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>410</v>
       </c>
@@ -2549,7 +2577,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>411</v>
       </c>
@@ -2575,7 +2603,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>412</v>
       </c>
@@ -2595,7 +2623,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>140</v>
       </c>
@@ -2615,7 +2643,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>140</v>
       </c>
@@ -2635,27 +2663,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K40" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L40" t="s">
+      <c r="L40" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>414</v>
       </c>
@@ -2675,27 +2703,27 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J42" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K42" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="L42" t="s">
+      <c r="L42" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>147</v>
       </c>
@@ -2712,7 +2740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>411</v>
       </c>
@@ -2738,7 +2766,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>394</v>
       </c>
@@ -2764,7 +2792,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>415</v>
       </c>
@@ -2784,7 +2812,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>416</v>
       </c>
@@ -2804,7 +2832,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>417</v>
       </c>
@@ -2824,7 +2852,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>418</v>
       </c>
@@ -2844,7 +2872,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>390</v>
       </c>
@@ -2858,7 +2886,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>398</v>
       </c>
@@ -2878,7 +2906,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>419</v>
       </c>
@@ -2898,7 +2926,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>420</v>
       </c>
@@ -2918,7 +2946,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>421</v>
       </c>
@@ -2938,7 +2966,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>159</v>
       </c>
@@ -2958,7 +2986,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>422</v>
       </c>
@@ -2978,27 +3006,27 @@
         <v>163</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="57" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
         <v>423</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J57" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="K57" t="s">
+      <c r="K57" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="L57" t="s">
+      <c r="L57" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>457</v>
       </c>
@@ -3018,7 +3046,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>167</v>
       </c>
@@ -3038,7 +3066,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>171</v>
       </c>
@@ -3058,7 +3086,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>172</v>
       </c>
@@ -3078,7 +3106,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>175</v>
       </c>
@@ -3104,7 +3132,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>457</v>
       </c>
@@ -3124,27 +3152,27 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="64" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="J64" t="s">
+      <c r="J64" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K64" t="s">
+      <c r="K64" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L64" t="s">
+      <c r="L64" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>183</v>
       </c>
@@ -3164,7 +3192,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>424</v>
       </c>
@@ -3184,7 +3212,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>425</v>
       </c>
@@ -3204,7 +3232,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>425</v>
       </c>
@@ -3224,7 +3252,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>426</v>
       </c>
@@ -3244,7 +3272,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>427</v>
       </c>
@@ -3264,7 +3292,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>426</v>
       </c>
@@ -3284,7 +3312,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>428</v>
       </c>
@@ -3313,7 +3341,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>393</v>
       </c>
@@ -3333,7 +3361,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>429</v>
       </c>
@@ -3353,7 +3381,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>430</v>
       </c>
@@ -3376,7 +3404,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>431</v>
       </c>
@@ -3399,7 +3427,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>432</v>
       </c>
@@ -3419,7 +3447,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>192</v>
       </c>
@@ -3439,7 +3467,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>419</v>
       </c>
@@ -3459,7 +3487,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>433</v>
       </c>
@@ -3479,7 +3507,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>434</v>
       </c>
@@ -3499,7 +3527,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>435</v>
       </c>
@@ -3519,7 +3547,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>200</v>
       </c>
@@ -3539,7 +3567,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>436</v>
       </c>
@@ -3559,7 +3587,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>437</v>
       </c>
@@ -3579,7 +3607,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>438</v>
       </c>
@@ -3605,7 +3633,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>439</v>
       </c>
@@ -3631,7 +3659,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>440</v>
       </c>
@@ -3651,7 +3679,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>441</v>
       </c>
@@ -3671,27 +3699,27 @@
         <v>163</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="90" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="J90" t="s">
+      <c r="J90" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K90" t="s">
+      <c r="K90" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="L90" t="s">
+      <c r="L90" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>217</v>
       </c>
@@ -3711,7 +3739,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>220</v>
       </c>
@@ -3734,7 +3762,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>442</v>
       </c>
@@ -3754,7 +3782,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>421</v>
       </c>
@@ -3774,7 +3802,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>443</v>
       </c>
@@ -3794,7 +3822,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>444</v>
       </c>
@@ -3814,7 +3842,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>224</v>
       </c>
@@ -3834,7 +3862,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>415</v>
       </c>
@@ -3854,7 +3882,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>393</v>
       </c>
@@ -3874,7 +3902,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>227</v>
       </c>
@@ -3894,7 +3922,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>227</v>
       </c>
@@ -3914,7 +3942,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>227</v>
       </c>
@@ -3934,7 +3962,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>231</v>
       </c>
@@ -3954,7 +3982,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>231</v>
       </c>
@@ -3974,7 +4002,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>231</v>
       </c>
@@ -3988,7 +4016,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>231</v>
       </c>
@@ -4008,7 +4036,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>231</v>
       </c>
@@ -4028,7 +4056,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>231</v>
       </c>
@@ -4048,7 +4076,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>231</v>
       </c>
@@ -4068,7 +4096,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>445</v>
       </c>
@@ -4088,7 +4116,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>445</v>
       </c>
@@ -4108,7 +4136,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="112" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>446</v>
       </c>
@@ -4137,7 +4165,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>447</v>
       </c>
@@ -4157,27 +4185,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="114" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E114" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="J114" t="s">
+      <c r="J114" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="K114" t="s">
+      <c r="K114" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="L114" t="s">
+      <c r="L114" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>108</v>
       </c>
@@ -4197,7 +4225,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>108</v>
       </c>
@@ -4217,7 +4245,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>448</v>
       </c>
@@ -4237,7 +4265,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>414</v>
       </c>
@@ -4257,7 +4285,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>423</v>
       </c>
@@ -4277,7 +4305,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>241</v>
       </c>
@@ -4300,7 +4328,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>417</v>
       </c>
@@ -4320,7 +4348,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>436</v>
       </c>
@@ -4340,7 +4368,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>420</v>
       </c>
@@ -4360,7 +4388,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>245</v>
       </c>
@@ -4380,7 +4408,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>449</v>
       </c>
@@ -4400,7 +4428,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>449</v>
       </c>
@@ -4420,7 +4448,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>409</v>
       </c>
@@ -4440,7 +4468,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>250</v>
       </c>
@@ -4463,7 +4491,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>250</v>
       </c>
@@ -4483,7 +4511,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>450</v>
       </c>
@@ -4509,7 +4537,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>254</v>
       </c>
@@ -4529,7 +4557,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>257</v>
       </c>
@@ -4543,7 +4571,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>257</v>
       </c>
@@ -4563,7 +4591,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>451</v>
       </c>
@@ -4583,7 +4611,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>452</v>
       </c>
@@ -4603,7 +4631,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>262</v>
       </c>
@@ -4623,7 +4651,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>262</v>
       </c>
@@ -4643,7 +4671,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>262</v>
       </c>
@@ -4663,7 +4691,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>267</v>
       </c>
@@ -4683,7 +4711,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>388</v>
       </c>
@@ -4709,7 +4737,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>391</v>
       </c>
@@ -4729,7 +4757,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>435</v>
       </c>
@@ -4749,27 +4777,27 @@
         <v>199</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="143" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E143" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="J143" t="s">
+      <c r="J143" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K143" t="s">
+      <c r="K143" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L143" t="s">
+      <c r="L143" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>420</v>
       </c>
@@ -4789,7 +4817,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>270</v>
       </c>
@@ -4809,33 +4837,33 @@
         <v>92</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="146" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C146" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E146" t="s">
+      <c r="E146" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="F146" t="s">
+      <c r="F146" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="J146" t="s">
+      <c r="J146" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="K146" t="s">
+      <c r="K146" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="L146" t="s">
+      <c r="L146" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>275</v>
       </c>
@@ -4855,7 +4883,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>275</v>
       </c>
@@ -4875,7 +4903,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>275</v>
       </c>
@@ -4895,7 +4923,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>454</v>
       </c>
@@ -4921,7 +4949,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>455</v>
       </c>
@@ -4941,7 +4969,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>279</v>
       </c>
@@ -4961,7 +4989,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>394</v>
       </c>
@@ -4987,27 +5015,27 @@
         <v>55</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+    <row r="154" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B154" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="E154" t="s">
+      <c r="E154" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="J154" t="s">
+      <c r="J154" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="K154" t="s">
+      <c r="K154" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="L154" t="s">
+      <c r="L154" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>285</v>
       </c>
@@ -5027,7 +5055,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>456</v>
       </c>
@@ -5053,7 +5081,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>290</v>
       </c>
@@ -5073,7 +5101,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>290</v>
       </c>
@@ -5093,7 +5121,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>290</v>
       </c>
@@ -5113,7 +5141,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>406</v>
       </c>
@@ -5133,7 +5161,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>296</v>
       </c>
@@ -5153,7 +5181,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>441</v>
       </c>

</xml_diff>